<commit_message>
finish to assign todoList
</commit_message>
<xml_diff>
--- a/endpointAPI (copie).xlsx
+++ b/endpointAPI (copie).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="95">
   <si>
     <t xml:space="preserve">URI : groupe4/api</t>
   </si>
@@ -55,8 +55,7 @@
     <t xml:space="preserve">Retourne l’ensemble des users</t>
   </si>
   <si>
-    <t xml:space="preserve">FAIT
-</t>
+    <t xml:space="preserve">FAIT</t>
   </si>
   <si>
     <t xml:space="preserve">FD</t>
@@ -77,15 +76,15 @@
     <t xml:space="preserve">archive tous tous la base de donnée</t>
   </si>
   <si>
+    <t xml:space="preserve">à faire</t>
+  </si>
+  <si>
     <t xml:space="preserve">/users/userid</t>
   </si>
   <si>
     <t xml:space="preserve">Retourne le user dont l’id est userid</t>
   </si>
   <si>
-    <t xml:space="preserve">FAIT</t>
-  </si>
-  <si>
     <t xml:space="preserve">modifier l’utilisateur dont l’id est userid </t>
   </si>
   <si>
@@ -101,27 +100,27 @@
     <t xml:space="preserve">Retourne l’ensemble des posts du user dont l’id est userid</t>
   </si>
   <si>
+    <t xml:space="preserve">OD</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ajout d’un post par le user qui a l’id userid</t>
   </si>
   <si>
-    <t xml:space="preserve">OD</t>
-  </si>
-  <si>
     <t xml:space="preserve">Archive l’ensemble des posts du user dont l’id est userid</t>
   </si>
   <si>
     <t xml:space="preserve">archive tous les commentaires faits sur les postes du user dont l’id est userid</t>
   </si>
   <si>
+    <t xml:space="preserve">AD</t>
+  </si>
+  <si>
     <t xml:space="preserve">/users/userid/albums</t>
   </si>
   <si>
     <t xml:space="preserve">Retourne l’ensemble des albums du user dont l’id est userid</t>
   </si>
   <si>
-    <t xml:space="preserve">AD</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ajout d’un album par le user qui a l’id userid</t>
   </si>
   <si>
@@ -237,9 +236,6 @@
   </si>
   <si>
     <t xml:space="preserve">/photos/photoid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retourne la photo dont l’id est photoid</t>
   </si>
   <si>
     <t xml:space="preserve">modifie la photo qui a l’id photoid</t>
@@ -383,7 +379,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,6 +418,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF808080"/>
         <bgColor rgb="FF969696"/>
       </patternFill>
@@ -441,7 +443,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF383D3C"/>
-        <bgColor rgb="FF1C1C1C"/>
+        <bgColor rgb="FF333333"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF333333"/>
+        <bgColor rgb="FF383D3C"/>
       </patternFill>
     </fill>
   </fills>
@@ -479,7 +487,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -500,7 +508,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -512,6 +524,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -536,7 +552,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -552,11 +572,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -564,8 +592,8 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -627,14 +655,14 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF3465A4"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF111111"/>
       <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF111111"/>
       <rgbColor rgb="FF1C1C1C"/>
+      <rgbColor rgb="FF383D3C"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF55308D"/>
-      <rgbColor rgb="FF383D3C"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -645,10 +673,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:AMJ97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G93" activeCellId="0" sqref="G93"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="18.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -670,33 +698,34 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="5"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -705,35 +734,39 @@
       <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="12"/>
+      <c r="F3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="10"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
@@ -743,73 +776,100 @@
       <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F6" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9" t="s">
-        <v>18</v>
+      <c r="A8" s="10"/>
+      <c r="B8" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11" t="s">
         <v>20</v>
       </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="10"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="19" t="s">
         <v>23</v>
       </c>
+      <c r="F11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -818,122 +878,148 @@
       <c r="D13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="10"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="19" t="s">
         <v>29</v>
       </c>
+      <c r="F16" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9" t="s">
-        <v>30</v>
+      <c r="A18" s="10"/>
+      <c r="B18" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="17" t="s">
         <v>32</v>
       </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>27</v>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="10"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8"/>
-      <c r="B21" s="9"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="19" t="s">
         <v>35</v>
       </c>
+      <c r="F21" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -942,55 +1028,71 @@
       <c r="D23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="10"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="16" t="s">
+      <c r="E24" s="12"/>
+      <c r="F24" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="15" t="s">
-        <v>27</v>
+      <c r="G24" s="20" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8"/>
-      <c r="B25" s="9"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="10"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8"/>
-      <c r="B26" s="9"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="10"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9" t="s">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -999,108 +1101,128 @@
       <c r="D28" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>27</v>
+      <c r="E28" s="12"/>
+      <c r="F28" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8"/>
-      <c r="B29" s="9"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="10"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8"/>
-      <c r="B30" s="9"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="10"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="10"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="18"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="18"/>
-      <c r="B33" s="9" t="s">
+      <c r="A33" s="22"/>
+      <c r="B33" s="11" t="s">
         <v>43</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="10"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
     </row>
     <row r="34" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="18"/>
-      <c r="B34" s="9"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>27</v>
+      <c r="E34" s="12"/>
+      <c r="F34" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="18"/>
-      <c r="B35" s="9"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="10"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
     </row>
     <row r="36" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="18"/>
-      <c r="B36" s="9"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="13"/>
-      <c r="E36" s="10"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
     </row>
     <row r="37" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
     </row>
     <row r="38" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -1109,53 +1231,65 @@
       <c r="D38" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G38" s="12" t="s">
+      <c r="E38" s="12"/>
+      <c r="F38" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="13"/>
-      <c r="E39" s="10"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
     </row>
     <row r="40" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="13"/>
-      <c r="E40" s="10"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
     </row>
     <row r="41" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8"/>
-      <c r="B41" s="9"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E41" s="10"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="8"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
     </row>
     <row r="43" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8"/>
-      <c r="B43" s="9" t="s">
+      <c r="A43" s="10"/>
+      <c r="B43" s="11" t="s">
         <v>49</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1164,51 +1298,73 @@
       <c r="D43" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="10"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8"/>
-      <c r="B44" s="9"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D44" s="13"/>
-      <c r="E44" s="10"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
     </row>
     <row r="45" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="8"/>
-      <c r="B45" s="9"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E45" s="10"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="8"/>
-      <c r="B46" s="9"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="11"/>
       <c r="C46" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E46" s="10"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="19"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
     </row>
     <row r="48" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="11" t="s">
         <v>54</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -1217,35 +1373,39 @@
       <c r="D48" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E48" s="10"/>
-      <c r="F48" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G48" s="12" t="s">
+      <c r="E48" s="12"/>
+      <c r="F48" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
       <c r="C49" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="13"/>
-      <c r="E49" s="10"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
     </row>
     <row r="50" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
       <c r="C50" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D50" s="13"/>
-      <c r="E50" s="10"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
     </row>
     <row r="51" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
       <c r="C51" s="2" t="s">
         <v>15</v>
       </c>
@@ -1255,17 +1415,25 @@
       <c r="E51" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="F51" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" s="21" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="8"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
     </row>
     <row r="53" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8"/>
-      <c r="B53" s="9" t="s">
+      <c r="A53" s="10"/>
+      <c r="B53" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -1274,63 +1442,73 @@
       <c r="D53" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E53" s="10"/>
-      <c r="F53" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G53" s="17" t="s">
-        <v>32</v>
+      <c r="E53" s="12"/>
+      <c r="F53" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
       <c r="C54" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D54" s="13"/>
-      <c r="E54" s="10"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
     </row>
     <row r="55" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
+      <c r="A55" s="10"/>
+      <c r="B55" s="10"/>
       <c r="C55" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="10"/>
-      <c r="F55" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G55" s="17" t="s">
-        <v>32</v>
+      <c r="E55" s="12"/>
+      <c r="F55" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="21" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
       <c r="C56" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E56" s="16" t="s">
+      <c r="E56" s="19" t="s">
         <v>62</v>
       </c>
+      <c r="F56" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="8"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
+      <c r="A57" s="10"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
     </row>
     <row r="58" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="8"/>
-      <c r="B58" s="9" t="s">
+      <c r="A58" s="10"/>
+      <c r="B58" s="11" t="s">
         <v>63</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -1339,63 +1517,73 @@
       <c r="D58" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E58" s="10"/>
-      <c r="F58" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G58" s="17" t="s">
-        <v>32</v>
+      <c r="E58" s="12"/>
+      <c r="F58" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" s="21" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
       <c r="C59" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E59" s="10"/>
-      <c r="F59" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G59" s="15" t="s">
-        <v>27</v>
+      <c r="E59" s="12"/>
+      <c r="F59" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
       <c r="C60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D60" s="13"/>
-      <c r="E60" s="10"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
     </row>
     <row r="61" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
+      <c r="A61" s="10"/>
+      <c r="B61" s="10"/>
       <c r="C61" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="10"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="19"/>
-      <c r="B62" s="19"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
+      <c r="A62" s="23"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
     </row>
     <row r="63" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="11" t="s">
         <v>68</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -1404,367 +1592,479 @@
       <c r="D63" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E63" s="10"/>
-      <c r="F63" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G63" s="12" t="s">
+      <c r="E63" s="12"/>
+      <c r="F63" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G63" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="8"/>
-      <c r="B64" s="9"/>
+      <c r="A64" s="10"/>
+      <c r="B64" s="11"/>
       <c r="C64" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D64" s="13"/>
-      <c r="E64" s="10"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
     </row>
     <row r="65" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="8"/>
-      <c r="B65" s="9"/>
+      <c r="A65" s="10"/>
+      <c r="B65" s="11"/>
       <c r="C65" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="13"/>
-      <c r="E65" s="10"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
     </row>
     <row r="66" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="8"/>
-      <c r="B66" s="9"/>
+      <c r="A66" s="10"/>
+      <c r="B66" s="11"/>
       <c r="C66" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E66" s="10"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" s="20" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="8"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
     </row>
     <row r="68" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="8"/>
-      <c r="B68" s="9" t="s">
+      <c r="A68" s="10"/>
+      <c r="B68" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E68" s="10"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
     </row>
     <row r="69" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="8"/>
-      <c r="B69" s="9"/>
+      <c r="A69" s="10"/>
+      <c r="B69" s="11"/>
       <c r="C69" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D69" s="13"/>
-      <c r="E69" s="10"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
     </row>
     <row r="70" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="8"/>
-      <c r="B70" s="9"/>
+      <c r="A70" s="10"/>
+      <c r="B70" s="11"/>
       <c r="C70" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E70" s="10"/>
+        <v>72</v>
+      </c>
+      <c r="E70" s="12"/>
+      <c r="F70" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G70" s="20" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="8"/>
-      <c r="B71" s="9"/>
+      <c r="A71" s="10"/>
+      <c r="B71" s="11"/>
       <c r="C71" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D71" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E71" s="25"/>
+      <c r="F71" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="23"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="24"/>
+    </row>
+    <row r="73" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E71" s="20"/>
-    </row>
-    <row r="72" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="19"/>
-      <c r="B72" s="19"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
-    </row>
-    <row r="73" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="8" t="s">
+      <c r="B73" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E73" s="10"/>
-      <c r="F73" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G73" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E73" s="12"/>
+      <c r="F73" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G73" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="8"/>
-      <c r="B74" s="9"/>
+      <c r="A74" s="10"/>
+      <c r="B74" s="11"/>
       <c r="C74" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D74" s="13"/>
-      <c r="E74" s="10"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
     </row>
     <row r="75" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="8"/>
-      <c r="B75" s="9"/>
+      <c r="A75" s="10"/>
+      <c r="B75" s="11"/>
       <c r="C75" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D75" s="13"/>
-      <c r="E75" s="10"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
     </row>
     <row r="76" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="8"/>
-      <c r="B76" s="9"/>
+      <c r="A76" s="10"/>
+      <c r="B76" s="11"/>
       <c r="C76" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D76" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E76" s="12"/>
+      <c r="F76" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G76" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="10"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
+    </row>
+    <row r="78" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="10"/>
+      <c r="B78" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="E76" s="10"/>
-    </row>
-    <row r="77" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="8"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-    </row>
-    <row r="78" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="8"/>
-      <c r="B78" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E78" s="10"/>
+        <v>79</v>
+      </c>
+      <c r="E78" s="12"/>
+      <c r="F78" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G78" s="21" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="8"/>
-      <c r="B79" s="9"/>
+      <c r="A79" s="10"/>
+      <c r="B79" s="11"/>
       <c r="C79" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D79" s="13"/>
-      <c r="E79" s="10"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
     </row>
     <row r="80" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="8"/>
-      <c r="B80" s="9"/>
+      <c r="A80" s="10"/>
+      <c r="B80" s="11"/>
       <c r="C80" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E80" s="10"/>
+        <v>80</v>
+      </c>
+      <c r="E80" s="12"/>
+      <c r="F80" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G80" s="20" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="8"/>
-      <c r="B81" s="9"/>
+      <c r="A81" s="10"/>
+      <c r="B81" s="11"/>
       <c r="C81" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D81" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E81" s="25"/>
+      <c r="F81" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G81" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="23"/>
+      <c r="B82" s="23"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="24"/>
+    </row>
+    <row r="83" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E81" s="20"/>
-    </row>
-    <row r="82" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="19"/>
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19"/>
-    </row>
-    <row r="83" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="8" t="s">
+      <c r="B83" s="11" t="s">
         <v>83</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>84</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E83" s="10"/>
-      <c r="F83" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G83" s="21" t="s">
-        <v>27</v>
+        <v>84</v>
+      </c>
+      <c r="E83" s="12"/>
+      <c r="F83" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G83" s="20" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="8"/>
-      <c r="B84" s="9"/>
+      <c r="A84" s="10"/>
+      <c r="B84" s="11"/>
       <c r="C84" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D84" s="13"/>
-      <c r="E84" s="10"/>
+      <c r="D84" s="15"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
     </row>
     <row r="85" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="8"/>
-      <c r="B85" s="9"/>
+      <c r="A85" s="10"/>
+      <c r="B85" s="11"/>
       <c r="C85" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D85" s="13"/>
-      <c r="E85" s="10"/>
-    </row>
-    <row r="86" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="8"/>
-      <c r="B86" s="9"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+    </row>
+    <row r="86" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="10"/>
+      <c r="B86" s="11"/>
       <c r="C86" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D86" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E86" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="F86" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G86" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="AMJ86" s="0"/>
+    </row>
+    <row r="87" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="10"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="17"/>
+      <c r="E87" s="17"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="18"/>
+    </row>
+    <row r="88" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="10"/>
+      <c r="B88" s="11" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="8"/>
-      <c r="B87" s="14"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-    </row>
-    <row r="88" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="8"/>
-      <c r="B88" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E88" s="10"/>
+        <v>88</v>
+      </c>
+      <c r="E88" s="12"/>
+      <c r="F88" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G88" s="21" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="8"/>
-      <c r="B89" s="9"/>
+      <c r="A89" s="10"/>
+      <c r="B89" s="11"/>
       <c r="C89" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D89" s="13"/>
-      <c r="E89" s="10"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
+      <c r="G89" s="12"/>
     </row>
     <row r="90" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="8"/>
-      <c r="B90" s="9"/>
+      <c r="A90" s="10"/>
+      <c r="B90" s="11"/>
       <c r="C90" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E90" s="10"/>
+        <v>89</v>
+      </c>
+      <c r="E90" s="12"/>
+      <c r="F90" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G90" s="20" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="8"/>
-      <c r="B91" s="9"/>
+      <c r="A91" s="10"/>
+      <c r="B91" s="11"/>
       <c r="C91" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D91" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E91" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="E91" s="16" t="s">
+      <c r="F91" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G91" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="17"/>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
+      <c r="F92" s="18"/>
+      <c r="G92" s="18"/>
+    </row>
+    <row r="93" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="11" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="14"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-    </row>
-    <row r="93" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="9" t="s">
-        <v>93</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E93" s="10"/>
-      <c r="F93" s="11" t="s">
-        <v>20</v>
+      <c r="D93" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E93" s="12"/>
+      <c r="F93" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G93" s="21" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="9"/>
+      <c r="B94" s="11"/>
       <c r="C94" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D94" s="13"/>
-      <c r="E94" s="10"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
     </row>
     <row r="95" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="9"/>
+      <c r="B95" s="11"/>
       <c r="C95" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D95" s="13"/>
-      <c r="E95" s="10"/>
+      <c r="D95" s="15"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
     </row>
     <row r="96" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="9"/>
+      <c r="B96" s="11"/>
       <c r="C96" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E96" s="20"/>
+        <v>94</v>
+      </c>
+      <c r="E96" s="25"/>
+      <c r="F96" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G96" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="19"/>
-      <c r="B97" s="19"/>
-      <c r="C97" s="19"/>
-      <c r="D97" s="19"/>
-      <c r="E97" s="19"/>
+      <c r="A97" s="23"/>
+      <c r="B97" s="23"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="46">

</xml_diff>

<commit_message>
finish to write route delete assign to FD
</commit_message>
<xml_diff>
--- a/endpointAPI (copie).xlsx
+++ b/endpointAPI (copie).xlsx
@@ -675,8 +675,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F66" activeCellId="0" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="18.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1490,8 +1490,8 @@
       <c r="E56" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F56" s="16" t="s">
-        <v>18</v>
+      <c r="F56" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="G56" s="14" t="s">
         <v>12</v>
@@ -1632,8 +1632,8 @@
         <v>70</v>
       </c>
       <c r="E66" s="12"/>
-      <c r="F66" s="16" t="s">
-        <v>18</v>
+      <c r="F66" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="G66" s="20" t="s">
         <v>26</v>
@@ -1988,8 +1988,8 @@
       <c r="E91" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="F91" s="16" t="s">
-        <v>18</v>
+      <c r="F91" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="G91" s="20" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
commit monday 23 may
</commit_message>
<xml_diff>
--- a/endpointAPI (copie).xlsx
+++ b/endpointAPI (copie).xlsx
@@ -675,8 +675,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="18.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -926,8 +926,8 @@
       <c r="E16" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="16" t="s">
-        <v>18</v>
+      <c r="F16" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="G16" s="21" t="s">
         <v>30</v>
@@ -1001,8 +1001,8 @@
       <c r="E21" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F21" s="13" t="s">
-        <v>11</v>
+      <c r="F21" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>26</v>
@@ -1029,8 +1029,8 @@
         <v>37</v>
       </c>
       <c r="E23" s="12"/>
-      <c r="F23" s="16" t="s">
-        <v>18</v>
+      <c r="F23" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="G23" s="21" t="s">
         <v>30</v>
@@ -1074,8 +1074,8 @@
         <v>39</v>
       </c>
       <c r="E26" s="12"/>
-      <c r="F26" s="13" t="s">
-        <v>11</v>
+      <c r="F26" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>12</v>
@@ -1344,8 +1344,8 @@
         <v>52</v>
       </c>
       <c r="E46" s="12"/>
-      <c r="F46" s="13" t="s">
-        <v>11</v>
+      <c r="F46" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="G46" s="20" t="s">
         <v>26</v>
@@ -1415,8 +1415,8 @@
       <c r="E51" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F51" s="16" t="s">
-        <v>18</v>
+      <c r="F51" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="G51" s="21" t="s">
         <v>30</v>
@@ -1632,8 +1632,8 @@
         <v>70</v>
       </c>
       <c r="E66" s="12"/>
-      <c r="F66" s="13" t="s">
-        <v>11</v>
+      <c r="F66" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="G66" s="20" t="s">
         <v>26</v>
@@ -1699,8 +1699,8 @@
         <v>73</v>
       </c>
       <c r="E71" s="25"/>
-      <c r="F71" s="16" t="s">
-        <v>18</v>
+      <c r="F71" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="G71" s="21" t="s">
         <v>30</v>
@@ -1796,8 +1796,8 @@
         <v>79</v>
       </c>
       <c r="E78" s="12"/>
-      <c r="F78" s="16" t="s">
-        <v>18</v>
+      <c r="F78" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="G78" s="21" t="s">
         <v>30</v>
@@ -1941,8 +1941,8 @@
         <v>88</v>
       </c>
       <c r="E88" s="12"/>
-      <c r="F88" s="16" t="s">
-        <v>18</v>
+      <c r="F88" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="G88" s="21" t="s">
         <v>30</v>
@@ -1988,8 +1988,8 @@
       <c r="E91" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="F91" s="13" t="s">
-        <v>11</v>
+      <c r="F91" s="16" t="s">
+        <v>18</v>
       </c>
       <c r="G91" s="20" t="s">
         <v>26</v>

</xml_diff>